<commit_message>
manually subscribed through 200. What about RSS?...
</commit_message>
<xml_diff>
--- a/resources/pharmaStocks.xlsx
+++ b/resources/pharmaStocks.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/montygash/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{555ED09B-F9A1-3844-A9F8-2F838ACBD982}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03116209-5581-B549-BD21-586AAE51667F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-3920" yWindow="-20940" windowWidth="20860" windowHeight="20940" xr2:uid="{794BBA13-F5D7-EB44-94F5-707D3C0EF582}"/>
+    <workbookView xWindow="2220" yWindow="500" windowWidth="20860" windowHeight="17500" xr2:uid="{794BBA13-F5D7-EB44-94F5-707D3C0EF582}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2021" uniqueCount="1292">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2121" uniqueCount="1292">
   <si>
     <t>AEMD</t>
   </si>
@@ -4264,8 +4264,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80CD966A-146C-5E4C-8921-A27243ED9F5A}">
   <dimension ref="A1:D640"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView tabSelected="1" topLeftCell="A174" workbookViewId="0">
+      <selection activeCell="C184" sqref="C184"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -5696,6 +5696,9 @@
       <c r="B102" t="s">
         <v>615</v>
       </c>
+      <c r="C102" t="s">
+        <v>1289</v>
+      </c>
       <c r="D102" t="s">
         <v>61</v>
       </c>
@@ -5707,6 +5710,9 @@
       <c r="B103" t="s">
         <v>616</v>
       </c>
+      <c r="C103" t="s">
+        <v>1289</v>
+      </c>
       <c r="D103" t="s">
         <v>61</v>
       </c>
@@ -5718,6 +5724,9 @@
       <c r="B104" t="s">
         <v>617</v>
       </c>
+      <c r="C104" t="s">
+        <v>1289</v>
+      </c>
       <c r="D104" t="s">
         <v>61</v>
       </c>
@@ -5729,6 +5738,9 @@
       <c r="B105" t="s">
         <v>618</v>
       </c>
+      <c r="C105" t="s">
+        <v>1289</v>
+      </c>
       <c r="D105" t="s">
         <v>61</v>
       </c>
@@ -5740,6 +5752,9 @@
       <c r="B106" t="s">
         <v>619</v>
       </c>
+      <c r="C106" t="s">
+        <v>1291</v>
+      </c>
       <c r="D106" t="s">
         <v>61</v>
       </c>
@@ -5751,6 +5766,9 @@
       <c r="B107" t="s">
         <v>620</v>
       </c>
+      <c r="C107" t="s">
+        <v>1289</v>
+      </c>
       <c r="D107" t="s">
         <v>61</v>
       </c>
@@ -5762,6 +5780,9 @@
       <c r="B108" t="s">
         <v>621</v>
       </c>
+      <c r="C108" t="s">
+        <v>1289</v>
+      </c>
       <c r="D108" t="s">
         <v>61</v>
       </c>
@@ -5773,6 +5794,9 @@
       <c r="B109" t="s">
         <v>622</v>
       </c>
+      <c r="C109" t="s">
+        <v>1291</v>
+      </c>
       <c r="D109" t="s">
         <v>61</v>
       </c>
@@ -5784,6 +5808,9 @@
       <c r="B110" t="s">
         <v>623</v>
       </c>
+      <c r="C110" t="s">
+        <v>1289</v>
+      </c>
       <c r="D110" t="s">
         <v>61</v>
       </c>
@@ -5795,6 +5822,9 @@
       <c r="B111" t="s">
         <v>624</v>
       </c>
+      <c r="C111" t="s">
+        <v>1289</v>
+      </c>
       <c r="D111" t="s">
         <v>61</v>
       </c>
@@ -5806,6 +5836,9 @@
       <c r="B112" t="s">
         <v>625</v>
       </c>
+      <c r="C112" t="s">
+        <v>1289</v>
+      </c>
       <c r="D112" t="s">
         <v>61</v>
       </c>
@@ -5817,6 +5850,9 @@
       <c r="B113" t="s">
         <v>626</v>
       </c>
+      <c r="C113" t="s">
+        <v>1289</v>
+      </c>
       <c r="D113" t="s">
         <v>61</v>
       </c>
@@ -5828,6 +5864,9 @@
       <c r="B114" t="s">
         <v>627</v>
       </c>
+      <c r="C114" t="s">
+        <v>1289</v>
+      </c>
       <c r="D114" t="s">
         <v>61</v>
       </c>
@@ -5839,6 +5878,9 @@
       <c r="B115" t="s">
         <v>628</v>
       </c>
+      <c r="C115" t="s">
+        <v>1289</v>
+      </c>
       <c r="D115" t="s">
         <v>61</v>
       </c>
@@ -5850,6 +5892,9 @@
       <c r="B116" t="s">
         <v>629</v>
       </c>
+      <c r="C116" t="s">
+        <v>1291</v>
+      </c>
       <c r="D116" t="s">
         <v>61</v>
       </c>
@@ -5861,6 +5906,9 @@
       <c r="B117" t="s">
         <v>630</v>
       </c>
+      <c r="C117" t="s">
+        <v>1291</v>
+      </c>
       <c r="D117" t="s">
         <v>61</v>
       </c>
@@ -5872,6 +5920,9 @@
       <c r="B118" t="s">
         <v>631</v>
       </c>
+      <c r="C118" t="s">
+        <v>1289</v>
+      </c>
       <c r="D118" t="s">
         <v>61</v>
       </c>
@@ -5883,6 +5934,9 @@
       <c r="B119" t="s">
         <v>632</v>
       </c>
+      <c r="C119" t="s">
+        <v>1289</v>
+      </c>
       <c r="D119" t="s">
         <v>61</v>
       </c>
@@ -5894,6 +5948,9 @@
       <c r="B120" t="s">
         <v>633</v>
       </c>
+      <c r="C120" t="s">
+        <v>1291</v>
+      </c>
       <c r="D120" t="s">
         <v>61</v>
       </c>
@@ -5905,6 +5962,9 @@
       <c r="B121" t="s">
         <v>635</v>
       </c>
+      <c r="C121" t="s">
+        <v>1289</v>
+      </c>
       <c r="D121" t="s">
         <v>61</v>
       </c>
@@ -5916,6 +5976,9 @@
       <c r="B122" t="s">
         <v>637</v>
       </c>
+      <c r="C122" t="s">
+        <v>1289</v>
+      </c>
       <c r="D122" t="s">
         <v>61</v>
       </c>
@@ -5927,6 +5990,9 @@
       <c r="B123" t="s">
         <v>639</v>
       </c>
+      <c r="C123" t="s">
+        <v>1289</v>
+      </c>
       <c r="D123" t="s">
         <v>61</v>
       </c>
@@ -5938,6 +6004,9 @@
       <c r="B124" t="s">
         <v>641</v>
       </c>
+      <c r="C124" t="s">
+        <v>1289</v>
+      </c>
       <c r="D124" t="s">
         <v>61</v>
       </c>
@@ -5949,6 +6018,9 @@
       <c r="B125" t="s">
         <v>643</v>
       </c>
+      <c r="C125" t="s">
+        <v>1291</v>
+      </c>
       <c r="D125" t="s">
         <v>61</v>
       </c>
@@ -5960,6 +6032,9 @@
       <c r="B126" t="s">
         <v>644</v>
       </c>
+      <c r="C126" t="s">
+        <v>1289</v>
+      </c>
       <c r="D126" t="s">
         <v>61</v>
       </c>
@@ -5971,6 +6046,9 @@
       <c r="B127" t="s">
         <v>645</v>
       </c>
+      <c r="C127" t="s">
+        <v>1289</v>
+      </c>
       <c r="D127" t="s">
         <v>61</v>
       </c>
@@ -5982,6 +6060,9 @@
       <c r="B128" t="s">
         <v>646</v>
       </c>
+      <c r="C128" t="s">
+        <v>1289</v>
+      </c>
       <c r="D128" t="s">
         <v>61</v>
       </c>
@@ -5993,6 +6074,9 @@
       <c r="B129" t="s">
         <v>647</v>
       </c>
+      <c r="C129" t="s">
+        <v>1289</v>
+      </c>
       <c r="D129" t="s">
         <v>61</v>
       </c>
@@ -6004,6 +6088,9 @@
       <c r="B130" t="s">
         <v>648</v>
       </c>
+      <c r="C130" t="s">
+        <v>1289</v>
+      </c>
       <c r="D130" t="s">
         <v>61</v>
       </c>
@@ -6015,6 +6102,9 @@
       <c r="B131" t="s">
         <v>650</v>
       </c>
+      <c r="C131" t="s">
+        <v>1291</v>
+      </c>
       <c r="D131" t="s">
         <v>61</v>
       </c>
@@ -6026,6 +6116,9 @@
       <c r="B132" t="s">
         <v>652</v>
       </c>
+      <c r="C132" t="s">
+        <v>1289</v>
+      </c>
       <c r="D132" t="s">
         <v>61</v>
       </c>
@@ -6037,6 +6130,9 @@
       <c r="B133" t="s">
         <v>653</v>
       </c>
+      <c r="C133" t="s">
+        <v>1289</v>
+      </c>
       <c r="D133" t="s">
         <v>61</v>
       </c>
@@ -6048,6 +6144,9 @@
       <c r="B134" t="s">
         <v>654</v>
       </c>
+      <c r="C134" t="s">
+        <v>1291</v>
+      </c>
       <c r="D134" t="s">
         <v>61</v>
       </c>
@@ -6059,6 +6158,9 @@
       <c r="B135" t="s">
         <v>655</v>
       </c>
+      <c r="C135" t="s">
+        <v>1289</v>
+      </c>
       <c r="D135" t="s">
         <v>95</v>
       </c>
@@ -6070,6 +6172,9 @@
       <c r="B136" t="s">
         <v>656</v>
       </c>
+      <c r="C136" t="s">
+        <v>1291</v>
+      </c>
       <c r="D136" t="s">
         <v>95</v>
       </c>
@@ -6081,6 +6186,9 @@
       <c r="B137" t="s">
         <v>657</v>
       </c>
+      <c r="C137" t="s">
+        <v>1289</v>
+      </c>
       <c r="D137" t="s">
         <v>95</v>
       </c>
@@ -6092,6 +6200,9 @@
       <c r="B138" t="s">
         <v>658</v>
       </c>
+      <c r="C138" t="s">
+        <v>1289</v>
+      </c>
       <c r="D138" t="s">
         <v>95</v>
       </c>
@@ -6103,6 +6214,9 @@
       <c r="B139" t="s">
         <v>659</v>
       </c>
+      <c r="C139" t="s">
+        <v>1289</v>
+      </c>
       <c r="D139" t="s">
         <v>95</v>
       </c>
@@ -6114,6 +6228,9 @@
       <c r="B140" t="s">
         <v>660</v>
       </c>
+      <c r="C140" t="s">
+        <v>1291</v>
+      </c>
       <c r="D140" t="s">
         <v>95</v>
       </c>
@@ -6125,6 +6242,9 @@
       <c r="B141" t="s">
         <v>661</v>
       </c>
+      <c r="C141" t="s">
+        <v>1289</v>
+      </c>
       <c r="D141" t="s">
         <v>95</v>
       </c>
@@ -6136,6 +6256,9 @@
       <c r="B142" t="s">
         <v>662</v>
       </c>
+      <c r="C142" t="s">
+        <v>1291</v>
+      </c>
       <c r="D142" t="s">
         <v>95</v>
       </c>
@@ -6147,6 +6270,9 @@
       <c r="B143" t="s">
         <v>663</v>
       </c>
+      <c r="C143" t="s">
+        <v>1289</v>
+      </c>
       <c r="D143" t="s">
         <v>95</v>
       </c>
@@ -6158,6 +6284,9 @@
       <c r="B144" t="s">
         <v>664</v>
       </c>
+      <c r="C144" t="s">
+        <v>1289</v>
+      </c>
       <c r="D144" t="s">
         <v>95</v>
       </c>
@@ -6169,6 +6298,9 @@
       <c r="B145" t="s">
         <v>665</v>
       </c>
+      <c r="C145" t="s">
+        <v>1289</v>
+      </c>
       <c r="D145" t="s">
         <v>95</v>
       </c>
@@ -6180,6 +6312,9 @@
       <c r="B146" t="s">
         <v>666</v>
       </c>
+      <c r="C146" t="s">
+        <v>1291</v>
+      </c>
       <c r="D146" t="s">
         <v>95</v>
       </c>
@@ -6191,6 +6326,9 @@
       <c r="B147" t="s">
         <v>667</v>
       </c>
+      <c r="C147" t="s">
+        <v>1289</v>
+      </c>
       <c r="D147" t="s">
         <v>95</v>
       </c>
@@ -6202,6 +6340,9 @@
       <c r="B148" t="s">
         <v>668</v>
       </c>
+      <c r="C148" t="s">
+        <v>1289</v>
+      </c>
       <c r="D148" t="s">
         <v>95</v>
       </c>
@@ -6213,6 +6354,9 @@
       <c r="B149" t="s">
         <v>669</v>
       </c>
+      <c r="C149" t="s">
+        <v>1289</v>
+      </c>
       <c r="D149" t="s">
         <v>95</v>
       </c>
@@ -6224,6 +6368,9 @@
       <c r="B150" t="s">
         <v>670</v>
       </c>
+      <c r="C150" t="s">
+        <v>1291</v>
+      </c>
       <c r="D150" t="s">
         <v>95</v>
       </c>
@@ -6235,6 +6382,9 @@
       <c r="B151" t="s">
         <v>671</v>
       </c>
+      <c r="C151" t="s">
+        <v>1289</v>
+      </c>
       <c r="D151" t="s">
         <v>95</v>
       </c>
@@ -6246,6 +6396,9 @@
       <c r="B152" t="s">
         <v>672</v>
       </c>
+      <c r="C152" t="s">
+        <v>1289</v>
+      </c>
       <c r="D152" t="s">
         <v>95</v>
       </c>
@@ -6257,6 +6410,9 @@
       <c r="B153" t="s">
         <v>674</v>
       </c>
+      <c r="C153" t="s">
+        <v>1289</v>
+      </c>
       <c r="D153" t="s">
         <v>95</v>
       </c>
@@ -6268,6 +6424,9 @@
       <c r="B154" t="s">
         <v>676</v>
       </c>
+      <c r="C154" t="s">
+        <v>1291</v>
+      </c>
       <c r="D154" t="s">
         <v>95</v>
       </c>
@@ -6279,6 +6438,9 @@
       <c r="B155" t="s">
         <v>678</v>
       </c>
+      <c r="C155" t="s">
+        <v>1289</v>
+      </c>
       <c r="D155" t="s">
         <v>95</v>
       </c>
@@ -6290,6 +6452,9 @@
       <c r="B156" t="s">
         <v>680</v>
       </c>
+      <c r="C156" t="s">
+        <v>1289</v>
+      </c>
       <c r="D156" t="s">
         <v>95</v>
       </c>
@@ -6301,6 +6466,9 @@
       <c r="B157" t="s">
         <v>681</v>
       </c>
+      <c r="C157" t="s">
+        <v>1289</v>
+      </c>
       <c r="D157" t="s">
         <v>114</v>
       </c>
@@ -6312,6 +6480,9 @@
       <c r="B158" t="s">
         <v>682</v>
       </c>
+      <c r="C158" t="s">
+        <v>1289</v>
+      </c>
       <c r="D158" t="s">
         <v>114</v>
       </c>
@@ -6323,6 +6494,9 @@
       <c r="B159" t="s">
         <v>683</v>
       </c>
+      <c r="C159" t="s">
+        <v>1291</v>
+      </c>
       <c r="D159" t="s">
         <v>114</v>
       </c>
@@ -6334,6 +6508,9 @@
       <c r="B160" t="s">
         <v>684</v>
       </c>
+      <c r="C160" t="s">
+        <v>1289</v>
+      </c>
       <c r="D160" t="s">
         <v>114</v>
       </c>
@@ -6345,6 +6522,9 @@
       <c r="B161" t="s">
         <v>685</v>
       </c>
+      <c r="C161" t="s">
+        <v>1289</v>
+      </c>
       <c r="D161" t="s">
         <v>114</v>
       </c>
@@ -6356,6 +6536,9 @@
       <c r="B162" t="s">
         <v>686</v>
       </c>
+      <c r="C162" t="s">
+        <v>1289</v>
+      </c>
       <c r="D162" t="s">
         <v>114</v>
       </c>
@@ -6367,6 +6550,9 @@
       <c r="B163" t="s">
         <v>687</v>
       </c>
+      <c r="C163" t="s">
+        <v>1291</v>
+      </c>
       <c r="D163" t="s">
         <v>114</v>
       </c>
@@ -6378,6 +6564,9 @@
       <c r="B164" t="s">
         <v>688</v>
       </c>
+      <c r="C164" t="s">
+        <v>1289</v>
+      </c>
       <c r="D164" t="s">
         <v>114</v>
       </c>
@@ -6389,6 +6578,9 @@
       <c r="B165" t="s">
         <v>689</v>
       </c>
+      <c r="C165" t="s">
+        <v>1289</v>
+      </c>
       <c r="D165" t="s">
         <v>114</v>
       </c>
@@ -6400,6 +6592,9 @@
       <c r="B166" t="s">
         <v>690</v>
       </c>
+      <c r="C166" t="s">
+        <v>1289</v>
+      </c>
       <c r="D166" t="s">
         <v>114</v>
       </c>
@@ -6411,6 +6606,9 @@
       <c r="B167" t="s">
         <v>691</v>
       </c>
+      <c r="C167" t="s">
+        <v>1289</v>
+      </c>
       <c r="D167" t="s">
         <v>114</v>
       </c>
@@ -6422,6 +6620,9 @@
       <c r="B168" t="s">
         <v>692</v>
       </c>
+      <c r="C168" t="s">
+        <v>1289</v>
+      </c>
       <c r="D168" t="s">
         <v>114</v>
       </c>
@@ -6433,6 +6634,9 @@
       <c r="B169" t="s">
         <v>693</v>
       </c>
+      <c r="C169" t="s">
+        <v>1289</v>
+      </c>
       <c r="D169" t="s">
         <v>114</v>
       </c>
@@ -6444,6 +6648,9 @@
       <c r="B170" t="s">
         <v>694</v>
       </c>
+      <c r="C170" t="s">
+        <v>1289</v>
+      </c>
       <c r="D170" t="s">
         <v>114</v>
       </c>
@@ -6455,6 +6662,9 @@
       <c r="B171" t="s">
         <v>695</v>
       </c>
+      <c r="C171" t="s">
+        <v>1291</v>
+      </c>
       <c r="D171" t="s">
         <v>114</v>
       </c>
@@ -6466,6 +6676,9 @@
       <c r="B172" t="s">
         <v>696</v>
       </c>
+      <c r="C172" t="s">
+        <v>1289</v>
+      </c>
       <c r="D172" t="s">
         <v>114</v>
       </c>
@@ -6477,6 +6690,9 @@
       <c r="B173" t="s">
         <v>697</v>
       </c>
+      <c r="C173" t="s">
+        <v>1289</v>
+      </c>
       <c r="D173" t="s">
         <v>114</v>
       </c>
@@ -6488,6 +6704,9 @@
       <c r="B174" t="s">
         <v>698</v>
       </c>
+      <c r="C174" t="s">
+        <v>1289</v>
+      </c>
       <c r="D174" t="s">
         <v>114</v>
       </c>
@@ -6499,6 +6718,9 @@
       <c r="B175" t="s">
         <v>699</v>
       </c>
+      <c r="C175" t="s">
+        <v>1289</v>
+      </c>
       <c r="D175" t="s">
         <v>114</v>
       </c>
@@ -6510,6 +6732,9 @@
       <c r="B176" t="s">
         <v>700</v>
       </c>
+      <c r="C176" t="s">
+        <v>1289</v>
+      </c>
       <c r="D176" t="s">
         <v>114</v>
       </c>
@@ -6521,6 +6746,9 @@
       <c r="B177" t="s">
         <v>701</v>
       </c>
+      <c r="C177" t="s">
+        <v>1289</v>
+      </c>
       <c r="D177" t="s">
         <v>114</v>
       </c>
@@ -6532,6 +6760,9 @@
       <c r="B178" t="s">
         <v>702</v>
       </c>
+      <c r="C178" t="s">
+        <v>1289</v>
+      </c>
       <c r="D178" t="s">
         <v>114</v>
       </c>
@@ -6543,6 +6774,9 @@
       <c r="B179" t="s">
         <v>703</v>
       </c>
+      <c r="C179" t="s">
+        <v>1289</v>
+      </c>
       <c r="D179" t="s">
         <v>114</v>
       </c>
@@ -6554,6 +6788,9 @@
       <c r="B180" t="s">
         <v>704</v>
       </c>
+      <c r="C180" t="s">
+        <v>1289</v>
+      </c>
       <c r="D180" t="s">
         <v>114</v>
       </c>
@@ -6565,6 +6802,9 @@
       <c r="B181" t="s">
         <v>705</v>
       </c>
+      <c r="C181" t="s">
+        <v>1289</v>
+      </c>
       <c r="D181" t="s">
         <v>114</v>
       </c>
@@ -6576,6 +6816,9 @@
       <c r="B182" t="s">
         <v>706</v>
       </c>
+      <c r="C182" t="s">
+        <v>1289</v>
+      </c>
       <c r="D182" t="s">
         <v>114</v>
       </c>
@@ -6587,6 +6830,9 @@
       <c r="B183" t="s">
         <v>707</v>
       </c>
+      <c r="C183" t="s">
+        <v>1289</v>
+      </c>
       <c r="D183" t="s">
         <v>114</v>
       </c>
@@ -6598,6 +6844,9 @@
       <c r="B184" t="s">
         <v>708</v>
       </c>
+      <c r="C184" t="s">
+        <v>1289</v>
+      </c>
       <c r="D184" t="s">
         <v>114</v>
       </c>
@@ -6609,6 +6858,9 @@
       <c r="B185" t="s">
         <v>709</v>
       </c>
+      <c r="C185" t="s">
+        <v>1289</v>
+      </c>
       <c r="D185" t="s">
         <v>114</v>
       </c>
@@ -6620,6 +6872,9 @@
       <c r="B186" t="s">
         <v>710</v>
       </c>
+      <c r="C186" t="s">
+        <v>1289</v>
+      </c>
       <c r="D186" t="s">
         <v>114</v>
       </c>
@@ -6631,6 +6886,9 @@
       <c r="B187" t="s">
         <v>711</v>
       </c>
+      <c r="C187" t="s">
+        <v>1289</v>
+      </c>
       <c r="D187" t="s">
         <v>114</v>
       </c>
@@ -6642,6 +6900,9 @@
       <c r="B188" t="s">
         <v>712</v>
       </c>
+      <c r="C188" t="s">
+        <v>1289</v>
+      </c>
       <c r="D188" t="s">
         <v>114</v>
       </c>
@@ -6653,6 +6914,9 @@
       <c r="B189" t="s">
         <v>713</v>
       </c>
+      <c r="C189" t="s">
+        <v>1289</v>
+      </c>
       <c r="D189" t="s">
         <v>114</v>
       </c>
@@ -6664,6 +6928,9 @@
       <c r="B190" t="s">
         <v>714</v>
       </c>
+      <c r="C190" t="s">
+        <v>1289</v>
+      </c>
       <c r="D190" t="s">
         <v>114</v>
       </c>
@@ -6675,6 +6942,9 @@
       <c r="B191" t="s">
         <v>715</v>
       </c>
+      <c r="C191" t="s">
+        <v>1289</v>
+      </c>
       <c r="D191" t="s">
         <v>114</v>
       </c>
@@ -6686,6 +6956,9 @@
       <c r="B192" t="s">
         <v>716</v>
       </c>
+      <c r="C192" t="s">
+        <v>1289</v>
+      </c>
       <c r="D192" t="s">
         <v>114</v>
       </c>
@@ -6697,6 +6970,9 @@
       <c r="B193" t="s">
         <v>717</v>
       </c>
+      <c r="C193" t="s">
+        <v>1289</v>
+      </c>
       <c r="D193" t="s">
         <v>114</v>
       </c>
@@ -6708,6 +6984,9 @@
       <c r="B194" t="s">
         <v>718</v>
       </c>
+      <c r="C194" t="s">
+        <v>1289</v>
+      </c>
       <c r="D194" t="s">
         <v>114</v>
       </c>
@@ -6719,6 +6998,9 @@
       <c r="B195" t="s">
         <v>719</v>
       </c>
+      <c r="C195" t="s">
+        <v>1289</v>
+      </c>
       <c r="D195" t="s">
         <v>114</v>
       </c>
@@ -6730,6 +7012,9 @@
       <c r="B196" t="s">
         <v>720</v>
       </c>
+      <c r="C196" t="s">
+        <v>1289</v>
+      </c>
       <c r="D196" t="s">
         <v>114</v>
       </c>
@@ -6741,6 +7026,9 @@
       <c r="B197" t="s">
         <v>721</v>
       </c>
+      <c r="C197" t="s">
+        <v>1289</v>
+      </c>
       <c r="D197" t="s">
         <v>114</v>
       </c>
@@ -6752,6 +7040,9 @@
       <c r="B198" t="s">
         <v>722</v>
       </c>
+      <c r="C198" t="s">
+        <v>1289</v>
+      </c>
       <c r="D198" t="s">
         <v>114</v>
       </c>
@@ -6763,6 +7054,9 @@
       <c r="B199" t="s">
         <v>723</v>
       </c>
+      <c r="C199" t="s">
+        <v>1289</v>
+      </c>
       <c r="D199" t="s">
         <v>114</v>
       </c>
@@ -6774,6 +7068,9 @@
       <c r="B200" t="s">
         <v>724</v>
       </c>
+      <c r="C200" t="s">
+        <v>1289</v>
+      </c>
       <c r="D200" t="s">
         <v>114</v>
       </c>
@@ -6784,6 +7081,9 @@
       </c>
       <c r="B201" t="s">
         <v>725</v>
+      </c>
+      <c r="C201" t="s">
+        <v>1289</v>
       </c>
       <c r="D201" t="s">
         <v>114</v>

</xml_diff>